<commit_message>
Update Excel template file and remove temporary file
- Update RosterLab-Free-Excel-Template.xlsx
- Remove temporary Excel file

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/public/images/excel/RosterLab-Free-Excel-Template.xlsx
+++ b/public/images/excel/RosterLab-Free-Excel-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryangreen/Documents/rosterlab-sanity-cms/public/images/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2CF012-3334-2741-AEC4-A02500FBB839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88E1E39-2C4D-8A42-9B17-999B9F89CEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -1782,6 +1782,82 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1811,82 +1887,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -2402,7 +2402,7 @@
   <dimension ref="A1:B75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2611,7 +2611,7 @@
       <pane xSplit="4" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="X3" sqref="X3"/>
+      <selection pane="bottomRight" activeCell="BE1" sqref="BE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2642,29 +2642,29 @@
   <sheetData>
     <row r="1" spans="1:58" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C1" s="23"/>
-      <c r="E1" s="114" t="s">
+      <c r="E1" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
       <c r="N1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="O1" s="12"/>
-      <c r="P1" s="108">
+      <c r="P1" s="127">
         <v>45887</v>
       </c>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="108"/>
-      <c r="S1" s="108"/>
-      <c r="T1" s="108"/>
-      <c r="U1" s="108"/>
+      <c r="Q1" s="127"/>
+      <c r="R1" s="127"/>
+      <c r="S1" s="127"/>
+      <c r="T1" s="127"/>
+      <c r="U1" s="127"/>
       <c r="W1" s="24" t="s">
         <v>49</v>
       </c>
@@ -2688,48 +2688,48 @@
     </row>
     <row r="2" spans="1:58" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D2" s="11"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="114"/>
-      <c r="L2" s="114"/>
-      <c r="M2" s="114"/>
-      <c r="N2" s="118" t="s">
+      <c r="E2" s="133"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="133"/>
+      <c r="H2" s="133"/>
+      <c r="I2" s="133"/>
+      <c r="J2" s="133"/>
+      <c r="K2" s="133"/>
+      <c r="L2" s="133"/>
+      <c r="M2" s="133"/>
+      <c r="N2" s="110" t="s">
         <v>48</v>
       </c>
-      <c r="O2" s="118"/>
-      <c r="P2" s="117">
-        <v>6</v>
-      </c>
-      <c r="Q2" s="117"/>
-      <c r="R2" s="117"/>
-      <c r="S2" s="117"/>
-      <c r="T2" s="117"/>
-      <c r="U2" s="117"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="109">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="109"/>
+      <c r="R2" s="109"/>
+      <c r="S2" s="109"/>
+      <c r="T2" s="109"/>
+      <c r="U2" s="109"/>
       <c r="AG2" s="1"/>
       <c r="AN2" s="12"/>
       <c r="AO2" s="12"/>
       <c r="AP2" s="10"/>
-      <c r="AQ2" s="134"/>
-      <c r="AR2" s="134"/>
-      <c r="AS2" s="134"/>
-      <c r="AT2" s="134"/>
-      <c r="AU2" s="134"/>
-      <c r="AV2" s="134"/>
-      <c r="AW2" s="134"/>
-      <c r="AX2" s="134"/>
+      <c r="AQ2" s="126"/>
+      <c r="AR2" s="126"/>
+      <c r="AS2" s="126"/>
+      <c r="AT2" s="126"/>
+      <c r="AU2" s="126"/>
+      <c r="AV2" s="126"/>
+      <c r="AW2" s="126"/>
+      <c r="AX2" s="126"/>
       <c r="AZ2" s="1"/>
       <c r="BA2" s="1"/>
       <c r="BB2" s="1"/>
     </row>
     <row r="3" spans="1:58" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="124"/>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
+      <c r="A3" s="116"/>
+      <c r="B3" s="116"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -2915,12 +2915,12 @@
       <c r="BB4" s="20"/>
     </row>
     <row r="5" spans="1:58" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="125" t="s">
+      <c r="A5" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="126"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="127"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="119"/>
       <c r="E5" s="28" t="s">
         <v>3</v>
       </c>
@@ -3090,12 +3090,12 @@
       </c>
     </row>
     <row r="6" spans="1:58" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="128" t="s">
+      <c r="A6" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="129"/>
-      <c r="C6" s="129"/>
-      <c r="D6" s="130"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="122"/>
       <c r="E6" s="30" t="str">
         <f t="shared" ref="E6:AT6" si="1">TEXT($P$1+E4,"DD")</f>
         <v>18</v>
@@ -3413,26 +3413,26 @@
       <c r="AT7" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="AV7" s="115" t="s">
+      <c r="AV7" s="134" t="s">
         <v>45</v>
       </c>
-      <c r="AW7" s="115"/>
-      <c r="AX7" s="115"/>
-      <c r="AZ7" s="116" t="s">
+      <c r="AW7" s="134"/>
+      <c r="AX7" s="134"/>
+      <c r="AZ7" s="108" t="s">
         <v>44</v>
       </c>
-      <c r="BA7" s="116"/>
-      <c r="BB7" s="116"/>
-      <c r="BC7" s="116"/>
-      <c r="BD7" s="116"/>
+      <c r="BA7" s="108"/>
+      <c r="BB7" s="108"/>
+      <c r="BC7" s="108"/>
+      <c r="BD7" s="108"/>
     </row>
     <row r="8" spans="1:58" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="132"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="133"/>
+      <c r="B8" s="124"/>
+      <c r="C8" s="124"/>
+      <c r="D8" s="125"/>
       <c r="E8" s="38"/>
       <c r="F8" s="39"/>
       <c r="G8" s="39"/>
@@ -6159,12 +6159,12 @@
       <c r="BB37" s="10"/>
     </row>
     <row r="38" spans="1:56" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="109" t="s">
+      <c r="A38" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="110"/>
-      <c r="C38" s="110"/>
-      <c r="D38" s="111"/>
+      <c r="B38" s="129"/>
+      <c r="C38" s="129"/>
+      <c r="D38" s="130"/>
       <c r="E38" s="75"/>
       <c r="F38" s="76"/>
       <c r="G38" s="76"/>
@@ -6213,10 +6213,10 @@
       <c r="B39" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="112" t="s">
+      <c r="C39" s="131" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="113"/>
+      <c r="D39" s="132"/>
       <c r="E39" s="84">
         <v>6</v>
       </c>
@@ -6349,10 +6349,10 @@
       <c r="B40" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="120" t="s">
+      <c r="C40" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="121"/>
+      <c r="D40" s="113"/>
       <c r="E40" s="84">
         <v>6</v>
       </c>
@@ -6485,10 +6485,10 @@
       <c r="B41" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="C41" s="122" t="s">
+      <c r="C41" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="123"/>
+      <c r="D41" s="115"/>
       <c r="E41" s="86">
         <v>4</v>
       </c>
@@ -6617,12 +6617,12 @@
       </c>
     </row>
     <row r="44" spans="1:56" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="119" t="s">
+      <c r="A44" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="B44" s="119"/>
-      <c r="C44" s="119"/>
-      <c r="D44" s="119"/>
+      <c r="B44" s="111"/>
+      <c r="C44" s="111"/>
+      <c r="D44" s="111"/>
     </row>
     <row r="45" spans="1:56" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="89"/>
@@ -7332,6 +7332,11 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="TAHbruZ1xoJnkSNUcs0WS3vC3lHju4pLSI5n+juIlhImrQYeGv26pdeNRd4IeQDyyE9m0ccao4cR76B62Ds1ew==" saltValue="wIJO3ugXLJ5Hg8ZQK72h5Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="16">
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E1:M2"/>
+    <mergeCell ref="AV7:AX7"/>
     <mergeCell ref="AZ7:BD7"/>
     <mergeCell ref="P2:U2"/>
     <mergeCell ref="N2:O2"/>
@@ -7343,11 +7348,6 @@
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="AQ2:AX2"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E1:M2"/>
-    <mergeCell ref="AV7:AX7"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="BC9:BC36">
@@ -7372,14 +7372,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a62baab7-6556-4ca5-b9c8-f6b0c8594c23" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5ac99154-28f2-45a3-9b22-3b52c7dcc4d7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7584,27 +7582,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a62baab7-6556-4ca5-b9c8-f6b0c8594c23" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5ac99154-28f2-45a3-9b22-3b52c7dcc4d7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{275CF408-5EE6-465D-9E55-B2D14DFD036B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401E8015-0FE6-4C3B-8F45-C630B5133B9D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="5ac99154-28f2-45a3-9b22-3b52c7dcc4d7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a62baab7-6556-4ca5-b9c8-f6b0c8594c23"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7629,9 +7620,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401E8015-0FE6-4C3B-8F45-C630B5133B9D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{275CF408-5EE6-465D-9E55-B2D14DFD036B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="5ac99154-28f2-45a3-9b22-3b52c7dcc4d7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a62baab7-6556-4ca5-b9c8-f6b0c8594c23"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>